<commit_message>
features.xlsx: for gpio, mention if pull resistor direction has its own register
</commit_message>
<xml_diff>
--- a/nodeCtrl/features.xlsx
+++ b/nodeCtrl/features.xlsx
@@ -4,7 +4,7 @@
   <fileVersion lastEdited="4" lowestEdited="4" rupBuild="3820"/>
   <workbookPr date1904="0"/>
   <bookViews>
-    <workbookView activeTab="1"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="GPIO" sheetId="1" r:id="rId1"/>
@@ -146,10 +146,16 @@
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalUp="0" diagonalDown="0">
+    <border>
       <start style="none">
         <color rgb="FFC7C7C7"/>
       </start>
+      <top style="none">
+        <color rgb="FFC7C7C7"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FFC7C7C7"/>
+      </bottom>
     </border>
     <border diagonalUp="0" diagonalDown="0">
       <start style="none">
@@ -354,10 +360,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0" tabSelected="1">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -368,11 +374,12 @@
     <col min="5" max="5" style="1" width="9.142308"/>
     <col min="6" max="6" style="1" width="14.4277" bestFit="1" customWidth="1"/>
     <col min="7" max="7" style="1" width="9.142308"/>
-    <col min="8" max="8" style="1" width="9.142308"/>
-    <col min="9" max="16384" style="1"/>
+    <col min="8" max="8" style="1" width="9.999399" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" style="1" width="25.14135" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="B1" t="str">
         <v># pins</v>
       </c>
@@ -394,8 +401,11 @@
       <c r="H1" t="str">
         <v>cap sense</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" t="str">
+        <v>Separate pull resistor reg?</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -417,8 +427,11 @@
       <c r="G2" t="str">
         <v>high, low</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="I2" t="str">
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -443,8 +456,11 @@
       <c r="H3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="I3" t="str">
+        <v>no, PxOUT</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
@@ -470,7 +486,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:9">
       <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
@@ -493,7 +509,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:9">
       <c r="A6" s="6" t="s">
         <v>11</v>
       </c>
@@ -516,7 +532,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:9">
       <c r="A7" s="7" t="s">
         <v>12</v>
       </c>
@@ -542,12 +558,12 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
   <hyperlinks>
-    <hyperlink ref="A6" r:id="rId1" tooltip="http://www.atmel.com/Images/doc8008.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
+    <hyperlink ref="A5" r:id="rId1" tooltip="http://www.atmel.com/images/Atmel-8271-8-bit-AVR-Microcontroller-ATmega48A-48PA-88A-88PA-168A-168PA-328-328P_datasheet_Complete.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
     <hyperlink ref="A2" r:id="rId2" tooltip="http://www.nxp.com/documents/data_sheet/LPC81XM.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
     <hyperlink ref="A3" r:id="rId3" tooltip="http://www.ti.com/lit/ug/slau144j/slau144j.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
-    <hyperlink ref="A5" r:id="rId4" tooltip="http://www.atmel.com/images/Atmel-8271-8-bit-AVR-Microcontroller-ATmega48A-48PA-88A-88PA-168A-168PA-328-328P_datasheet_Complete.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
+    <hyperlink ref="A7" r:id="rId4" tooltip="http://www.atmel.com/Images/Atmel-8495-8-bit-AVR-Microcontrollers-ATtiny441-ATtiny841_Datasheet.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
     <hyperlink ref="A4" r:id="rId5" tooltip="http://www.st.com/web/en/resource/technical/document/datasheet/DM00078075.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
-    <hyperlink ref="A7" r:id="rId6" tooltip="http://www.atmel.com/Images/Atmel-8495-8-bit-AVR-Microcontrollers-ATtiny441-ATtiny841_Datasheet.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
+    <hyperlink ref="A6" r:id="rId6" tooltip="http://www.atmel.com/Images/doc8008.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins left="1" right="1" top="1.667" bottom="1.667" header="1" footer="1"/>
@@ -562,7 +578,7 @@
   </sheetPr>
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -707,11 +723,11 @@
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
   <hyperlinks>
     <hyperlink ref="A5" r:id="rId1" tooltip="http://www.atmel.com/images/Atmel-8271-8-bit-AVR-Microcontroller-ATmega48A-48PA-88A-88PA-168A-168PA-328-328P_datasheet_Complete.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
-    <hyperlink ref="A2" r:id="rId2" tooltip="http://www.nxp.com/documents/data_sheet/LPC81XM.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
-    <hyperlink ref="A7" r:id="rId3" tooltip="http://www.atmel.com/Images/Atmel-8495-8-bit-AVR-Microcontrollers-ATtiny441-ATtiny841_Datasheet.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
-    <hyperlink ref="A6" r:id="rId4" tooltip="http://www.atmel.com/Images/doc8008.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
-    <hyperlink ref="A3" r:id="rId5" tooltip="http://www.ti.com/lit/ug/slau144j/slau144j.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
-    <hyperlink ref="A4" r:id="rId6" tooltip="http://www.st.com/web/en/resource/technical/document/datasheet/DM00078075.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
+    <hyperlink ref="A7" r:id="rId2" tooltip="http://www.atmel.com/Images/Atmel-8495-8-bit-AVR-Microcontrollers-ATtiny441-ATtiny841_Datasheet.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
+    <hyperlink ref="A3" r:id="rId3" tooltip="http://www.ti.com/lit/ug/slau144j/slau144j.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
+    <hyperlink ref="A4" r:id="rId4" tooltip="http://www.st.com/web/en/resource/technical/document/datasheet/DM00078075.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
+    <hyperlink ref="A6" r:id="rId5" tooltip="http://www.atmel.com/Images/doc8008.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
+    <hyperlink ref="A2" r:id="rId6" tooltip="http://www.nxp.com/documents/data_sheet/LPC81XM.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins left="1" right="1" top="1.667" bottom="1.667" header="1" footer="1"/>
@@ -925,12 +941,12 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
   <hyperlinks>
-    <hyperlink ref="A7" r:id="rId1" tooltip="http://www.atmel.com/Images/Atmel-8495-8-bit-AVR-Microcontrollers-ATtiny441-ATtiny841_Datasheet.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
-    <hyperlink ref="A3" r:id="rId2" tooltip="http://www.ti.com/lit/ug/slau144j/slau144j.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
-    <hyperlink ref="A4" r:id="rId3" tooltip="http://www.st.com/web/en/resource/technical/document/datasheet/DM00078075.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
-    <hyperlink ref="A2" r:id="rId4" tooltip="http://www.nxp.com/documents/data_sheet/LPC81XM.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
-    <hyperlink ref="A5" r:id="rId5" tooltip="http://www.atmel.com/images/Atmel-8271-8-bit-AVR-Microcontroller-ATmega48A-48PA-88A-88PA-168A-168PA-328-328P_datasheet_Complete.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
-    <hyperlink ref="A6" r:id="rId6" tooltip="http://www.atmel.com/Images/doc8008.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
+    <hyperlink ref="A2" r:id="rId1" tooltip="http://www.nxp.com/documents/data_sheet/LPC81XM.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
+    <hyperlink ref="A4" r:id="rId2" tooltip="http://www.st.com/web/en/resource/technical/document/datasheet/DM00078075.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
+    <hyperlink ref="A3" r:id="rId3" tooltip="http://www.ti.com/lit/ug/slau144j/slau144j.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
+    <hyperlink ref="A5" r:id="rId4" tooltip="http://www.atmel.com/images/Atmel-8271-8-bit-AVR-Microcontroller-ATmega48A-48PA-88A-88PA-168A-168PA-328-328P_datasheet_Complete.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
+    <hyperlink ref="A6" r:id="rId5" tooltip="http://www.atmel.com/Images/doc8008.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
+    <hyperlink ref="A7" r:id="rId6" tooltip="http://www.atmel.com/Images/Atmel-8495-8-bit-AVR-Microcontrollers-ATtiny441-ATtiny841_Datasheet.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins left="1" right="1" top="1.667" bottom="1.667" header="1" footer="1"/>
@@ -988,12 +1004,12 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" tooltip="http://www.ti.com/lit/ug/slau144j/slau144j.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
-    <hyperlink ref="A2" r:id="rId2" tooltip="http://www.nxp.com/documents/data_sheet/LPC81XM.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
-    <hyperlink ref="A5" r:id="rId3" tooltip="http://www.atmel.com/images/Atmel-8271-8-bit-AVR-Microcontroller-ATmega48A-48PA-88A-88PA-168A-168PA-328-328P_datasheet_Complete.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
-    <hyperlink ref="A4" r:id="rId4" tooltip="http://www.st.com/web/en/resource/technical/document/datasheet/DM00078075.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
-    <hyperlink ref="A7" r:id="rId5" tooltip="http://www.atmel.com/Images/Atmel-8495-8-bit-AVR-Microcontrollers-ATtiny441-ATtiny841_Datasheet.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
-    <hyperlink ref="A6" r:id="rId6" tooltip="http://www.atmel.com/Images/doc8008.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
+    <hyperlink ref="A6" r:id="rId1" tooltip="http://www.atmel.com/Images/doc8008.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
+    <hyperlink ref="A7" r:id="rId2" tooltip="http://www.atmel.com/Images/Atmel-8495-8-bit-AVR-Microcontrollers-ATtiny441-ATtiny841_Datasheet.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
+    <hyperlink ref="A3" r:id="rId3" tooltip="http://www.ti.com/lit/ug/slau144j/slau144j.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
+    <hyperlink ref="A5" r:id="rId4" tooltip="http://www.atmel.com/images/Atmel-8271-8-bit-AVR-Microcontroller-ATmega48A-48PA-88A-88PA-168A-168PA-328-328P_datasheet_Complete.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
+    <hyperlink ref="A2" r:id="rId5" tooltip="http://www.nxp.com/documents/data_sheet/LPC81XM.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
+    <hyperlink ref="A4" r:id="rId6" tooltip="http://www.st.com/web/en/resource/technical/document/datasheet/DM00078075.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins left="1" right="1" top="1.667" bottom="1.667" header="1" footer="1"/>
@@ -1051,12 +1067,12 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
   <hyperlinks>
-    <hyperlink ref="A5" r:id="rId1" tooltip="http://www.atmel.com/images/Atmel-8271-8-bit-AVR-Microcontroller-ATmega48A-48PA-88A-88PA-168A-168PA-328-328P_datasheet_Complete.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
-    <hyperlink ref="A7" r:id="rId2" tooltip="http://www.atmel.com/Images/Atmel-8495-8-bit-AVR-Microcontrollers-ATtiny441-ATtiny841_Datasheet.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
+    <hyperlink ref="A6" r:id="rId1" tooltip="http://www.atmel.com/Images/doc8008.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
+    <hyperlink ref="A5" r:id="rId2" tooltip="http://www.atmel.com/images/Atmel-8271-8-bit-AVR-Microcontroller-ATmega48A-48PA-88A-88PA-168A-168PA-328-328P_datasheet_Complete.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
     <hyperlink ref="A2" r:id="rId3" tooltip="http://www.nxp.com/documents/data_sheet/LPC81XM.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
-    <hyperlink ref="A3" r:id="rId4" tooltip="http://www.ti.com/lit/ug/slau144j/slau144j.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
-    <hyperlink ref="A4" r:id="rId5" tooltip="http://www.st.com/web/en/resource/technical/document/datasheet/DM00078075.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
-    <hyperlink ref="A6" r:id="rId6" tooltip="http://www.atmel.com/Images/doc8008.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
+    <hyperlink ref="A4" r:id="rId4" tooltip="http://www.st.com/web/en/resource/technical/document/datasheet/DM00078075.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
+    <hyperlink ref="A3" r:id="rId5" tooltip="http://www.ti.com/lit/ug/slau144j/slau144j.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
+    <hyperlink ref="A7" r:id="rId6" tooltip="http://www.atmel.com/Images/Atmel-8495-8-bit-AVR-Microcontrollers-ATtiny441-ATtiny841_Datasheet.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins left="1" right="1" top="1.667" bottom="1.667" header="1" footer="1"/>
@@ -1114,12 +1130,12 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
   <hyperlinks>
-    <hyperlink ref="A7" r:id="rId1" tooltip="http://www.atmel.com/Images/Atmel-8495-8-bit-AVR-Microcontrollers-ATtiny441-ATtiny841_Datasheet.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
-    <hyperlink ref="A4" r:id="rId2" tooltip="http://www.st.com/web/en/resource/technical/document/datasheet/DM00078075.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
+    <hyperlink ref="A5" r:id="rId1" tooltip="http://www.atmel.com/images/Atmel-8271-8-bit-AVR-Microcontroller-ATmega48A-48PA-88A-88PA-168A-168PA-328-328P_datasheet_Complete.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
+    <hyperlink ref="A2" r:id="rId2" tooltip="http://www.nxp.com/documents/data_sheet/LPC81XM.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
     <hyperlink ref="A6" r:id="rId3" tooltip="http://www.atmel.com/Images/doc8008.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
     <hyperlink ref="A3" r:id="rId4" tooltip="http://www.ti.com/lit/ug/slau144j/slau144j.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
-    <hyperlink ref="A2" r:id="rId5" tooltip="http://www.nxp.com/documents/data_sheet/LPC81XM.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
-    <hyperlink ref="A5" r:id="rId6" tooltip="http://www.atmel.com/images/Atmel-8271-8-bit-AVR-Microcontroller-ATmega48A-48PA-88A-88PA-168A-168PA-328-328P_datasheet_Complete.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
+    <hyperlink ref="A4" r:id="rId5" tooltip="http://www.st.com/web/en/resource/technical/document/datasheet/DM00078075.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
+    <hyperlink ref="A7" r:id="rId6" tooltip="http://www.atmel.com/Images/Atmel-8495-8-bit-AVR-Microcontrollers-ATtiny441-ATtiny841_Datasheet.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins left="1" right="1" top="1.667" bottom="1.667" header="1" footer="1"/>
@@ -1177,12 +1193,12 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" tooltip="http://www.nxp.com/documents/data_sheet/LPC81XM.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
-    <hyperlink ref="A4" r:id="rId2" tooltip="http://www.st.com/web/en/resource/technical/document/datasheet/DM00078075.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
-    <hyperlink ref="A6" r:id="rId3" tooltip="http://www.atmel.com/Images/doc8008.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
-    <hyperlink ref="A7" r:id="rId4" tooltip="http://www.atmel.com/Images/Atmel-8495-8-bit-AVR-Microcontrollers-ATtiny441-ATtiny841_Datasheet.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
-    <hyperlink ref="A3" r:id="rId5" tooltip="http://www.ti.com/lit/ug/slau144j/slau144j.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
-    <hyperlink ref="A5" r:id="rId6" tooltip="http://www.atmel.com/images/Atmel-8271-8-bit-AVR-Microcontroller-ATmega48A-48PA-88A-88PA-168A-168PA-328-328P_datasheet_Complete.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
+    <hyperlink ref="A6" r:id="rId1" tooltip="http://www.atmel.com/Images/doc8008.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
+    <hyperlink ref="A7" r:id="rId2" tooltip="http://www.atmel.com/Images/Atmel-8495-8-bit-AVR-Microcontrollers-ATtiny441-ATtiny841_Datasheet.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
+    <hyperlink ref="A5" r:id="rId3" tooltip="http://www.atmel.com/images/Atmel-8271-8-bit-AVR-Microcontroller-ATmega48A-48PA-88A-88PA-168A-168PA-328-328P_datasheet_Complete.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
+    <hyperlink ref="A4" r:id="rId4" tooltip="http://www.st.com/web/en/resource/technical/document/datasheet/DM00078075.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
+    <hyperlink ref="A2" r:id="rId5" tooltip="http://www.nxp.com/documents/data_sheet/LPC81XM.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
+    <hyperlink ref="A3" r:id="rId6" tooltip="http://www.ti.com/lit/ug/slau144j/slau144j.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins left="1" right="1" top="1.667" bottom="1.667" header="1" footer="1"/>
@@ -1241,11 +1257,11 @@
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
   <hyperlinks>
     <hyperlink ref="A4" r:id="rId1" tooltip="http://www.st.com/web/en/resource/technical/document/datasheet/DM00078075.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
-    <hyperlink ref="A7" r:id="rId2" tooltip="http://www.atmel.com/Images/Atmel-8495-8-bit-AVR-Microcontrollers-ATtiny441-ATtiny841_Datasheet.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
-    <hyperlink ref="A6" r:id="rId3" tooltip="http://www.atmel.com/Images/doc8008.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
+    <hyperlink ref="A2" r:id="rId2" tooltip="http://www.nxp.com/documents/data_sheet/LPC81XM.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
+    <hyperlink ref="A3" r:id="rId3" tooltip="http://www.ti.com/lit/ug/slau144j/slau144j.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
     <hyperlink ref="A5" r:id="rId4" tooltip="http://www.atmel.com/images/Atmel-8271-8-bit-AVR-Microcontroller-ATmega48A-48PA-88A-88PA-168A-168PA-328-328P_datasheet_Complete.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
-    <hyperlink ref="A2" r:id="rId5" tooltip="http://www.nxp.com/documents/data_sheet/LPC81XM.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
-    <hyperlink ref="A3" r:id="rId6" tooltip="http://www.ti.com/lit/ug/slau144j/slau144j.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
+    <hyperlink ref="A7" r:id="rId5" tooltip="http://www.atmel.com/Images/Atmel-8495-8-bit-AVR-Microcontrollers-ATtiny441-ATtiny841_Datasheet.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
+    <hyperlink ref="A6" r:id="rId6" tooltip="http://www.atmel.com/Images/doc8008.pdf&#10;Left click once to follow this link.&#10;Middle click once to select this cell"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins left="1" right="1" top="1.667" bottom="1.667" header="1" footer="1"/>

</xml_diff>